<commit_message>
added values in excel
</commit_message>
<xml_diff>
--- a/data/relationships/relative_relations.xlsx
+++ b/data/relationships/relative_relations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanda\Work\spatial_computing\data\relationships\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E186950-A8BB-418B-A77C-EE152BE04D72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B00512E3-8600-4D28-8783-798C724C382C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{CF23ADFC-7355-454C-8301-86BE885D5D97}"/>
   </bookViews>
@@ -34,13 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="30">
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="28">
   <si>
     <t>student_housing</t>
   </si>
@@ -764,7 +758,7 @@
   <dimension ref="A1:AC29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AI20" sqref="AI20"/>
+      <selection activeCell="AE31" sqref="AE31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -772,93 +766,93 @@
     <row r="1" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="S1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="T1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="U1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="V1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="W1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="X1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="Y1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="11" t="s">
+      <c r="Z1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="AA1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="AB1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AC1" s="16" t="s">
         <v>27</v>
-      </c>
-      <c r="AB1" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="AC1" s="16" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" s="3">
         <v>0.4</v>
@@ -947,7 +941,7 @@
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3" s="7">
         <v>1</v>
@@ -1036,7 +1030,7 @@
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" s="7">
         <v>0</v>
@@ -1107,10 +1101,10 @@
       <c r="X4" s="9">
         <v>0</v>
       </c>
-      <c r="Y4" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="9" t="s">
+      <c r="Y4" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="9">
         <v>0</v>
       </c>
       <c r="AA4" s="9">
@@ -1125,7 +1119,7 @@
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5" s="7">
         <v>0</v>
@@ -1214,7 +1208,7 @@
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6" s="7">
         <v>0</v>
@@ -1303,7 +1297,7 @@
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" s="7">
         <v>0</v>
@@ -1392,7 +1386,7 @@
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B8" s="7">
         <v>0</v>
@@ -1481,7 +1475,7 @@
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9" s="7">
         <v>0</v>
@@ -1570,7 +1564,7 @@
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10" s="7">
         <v>0</v>
@@ -1659,7 +1653,7 @@
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11" s="7">
         <v>0</v>
@@ -1748,7 +1742,7 @@
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="7">
         <v>1</v>
@@ -1837,7 +1831,7 @@
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" s="7">
         <v>0</v>
@@ -1926,7 +1920,7 @@
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" s="7">
         <v>0</v>
@@ -2015,7 +2009,7 @@
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="7">
         <v>0</v>
@@ -2104,7 +2098,7 @@
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" s="7">
         <v>0</v>
@@ -2193,7 +2187,7 @@
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="7">
         <v>0</v>
@@ -2282,7 +2276,7 @@
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" s="7">
         <v>0</v>
@@ -2371,7 +2365,7 @@
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" s="7">
         <v>0</v>
@@ -2460,7 +2454,7 @@
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B20" s="7">
         <v>0</v>
@@ -2549,7 +2543,7 @@
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B21" s="7">
         <v>0</v>
@@ -2638,7 +2632,7 @@
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22" s="7">
         <v>0</v>
@@ -2727,7 +2721,7 @@
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B23" s="7">
         <v>0</v>
@@ -2816,7 +2810,7 @@
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B24" s="12">
         <v>0</v>
@@ -2884,8 +2878,8 @@
       <c r="W24" s="13">
         <v>1</v>
       </c>
-      <c r="X24" s="14" t="s">
-        <v>1</v>
+      <c r="X24" s="14">
+        <v>0</v>
       </c>
       <c r="Y24" s="13">
         <v>1</v>
@@ -2905,7 +2899,7 @@
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B25" s="7">
         <v>0</v>
@@ -2913,7 +2907,7 @@
       <c r="C25" s="9">
         <v>0</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D25" s="9">
         <v>0</v>
       </c>
       <c r="E25" s="9">
@@ -2994,7 +2988,7 @@
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B26" s="7">
         <v>0</v>
@@ -3002,7 +2996,7 @@
       <c r="C26" s="9">
         <v>0</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="D26" s="9">
         <v>0</v>
       </c>
       <c r="E26" s="9">
@@ -3011,7 +3005,7 @@
       <c r="F26" s="9">
         <v>0</v>
       </c>
-      <c r="G26" s="9" t="s">
+      <c r="G26" s="9">
         <v>0</v>
       </c>
       <c r="H26" s="9">
@@ -3083,7 +3077,7 @@
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B27" s="7">
         <v>0</v>
@@ -3172,7 +3166,7 @@
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B28" s="7">
         <v>0</v>
@@ -3261,7 +3255,7 @@
     </row>
     <row r="29" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B29" s="9">
         <v>0</v>

</xml_diff>